<commit_message>
TypeCheck implemented. Small modifications to Syntax to allow for Bang types to carry underlying type information.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-05september2016.xlsx
+++ b/time-labor/week-of-05september2016.xlsx
@@ -59,6 +59,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t xml:space="preserve">Weekly Time Record</t>
   </si>
@@ -157,9 +158,6 @@
   </si>
   <si>
     <t xml:space="preserve">Thursday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 – </t>
   </si>
   <si>
     <t xml:space="preserve">Friday</t>
@@ -204,6 +202,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -226,12 +225,14 @@
       <color rgb="FF7F7F7F"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="22"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -239,28 +240,33 @@
       <color rgb="FF37525F"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF7F7F7F"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF7F7F7F"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -268,17 +274,20 @@
       <color rgb="FF6896CE"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="9"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -632,7 +641,7 @@
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.6326530612245"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -925,13 +934,17 @@
       <c r="B16" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="19" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="D16" s="20" t="n">
+        <v>0.666666666666667</v>
+      </c>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="21" t="n">
         <f aca="false">IF((((D16-C16)+(F16-E16))*24)&gt;8,8,((D16-C16)+(F16-E16))*24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H16" s="21" t="n">
         <f aca="false">IF(((D16-C16)+(F16-E16))*24&gt;8,((D16-C16)+(F16-E16))*24-8,0)</f>
@@ -940,21 +953,23 @@
       <c r="I16" s="22"/>
       <c r="J16" s="23"/>
       <c r="K16" s="24"/>
-      <c r="L16" s="0" t="s">
-        <v>29</v>
-      </c>
+      <c r="L16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+        <v>29</v>
+      </c>
+      <c r="C17" s="19" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="D17" s="20" t="n">
+        <v>0.458333333333333</v>
+      </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21" t="n">
         <f aca="false">IF((((D17-C17)+(F17-E17))*24)&gt;8,8,((D17-C17)+(F17-E17))*24)</f>
-        <v>0</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="H17" s="21" t="n">
         <f aca="false">IF(((D17-C17)+(F17-E17))*24&gt;8,((D17-C17)+(F17-E17))*24-8,0)</f>
@@ -967,15 +982,19 @@
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+        <v>30</v>
+      </c>
+      <c r="C18" s="19" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D18" s="20" t="n">
+        <v>0.791666666666667</v>
+      </c>
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
       <c r="G18" s="21" t="n">
         <f aca="false">IF((((D18-C18)+(F18-E18))*24)&gt;8,8,((D18-C18)+(F18-E18))*24)</f>
-        <v>0</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="H18" s="21" t="n">
         <f aca="false">IF(((D18-C18)+(F18-E18))*24&gt;8,((D18-C18)+(F18-E18))*24-8,0)</f>
@@ -988,15 +1007,19 @@
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
+        <v>31</v>
+      </c>
+      <c r="C19" s="19" t="n">
+        <v>0.874305555555556</v>
+      </c>
+      <c r="D19" s="20" t="n">
+        <v>0.999305555555556</v>
+      </c>
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
       <c r="G19" s="21" t="n">
         <f aca="false">IF((((D19-C19)+(F19-E19))*24)&gt;8,8,((D19-C19)+(F19-E19))*24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19" s="21" t="n">
         <f aca="false">IF(((D19-C19)+(F19-E19))*24&gt;8,((D19-C19)+(F19-E19))*24-8,0)</f>
@@ -1013,11 +1036,11 @@
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
       <c r="F20" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1040,7 +1063,7 @@
       <c r="D21" s="26"/>
       <c r="E21" s="25"/>
       <c r="F21" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G21" s="28" t="n">
         <v>10</v>
@@ -1063,7 +1086,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1079,7 +1102,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="L22" s="0"/>
     </row>
@@ -1110,14 +1133,14 @@
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
       <c r="K25" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1130,14 +1153,14 @@
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="34"/>
       <c r="K27" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>